<commit_message>
Correcciones para traer datos de sprint, code smell y la deuda técnica
</commit_message>
<xml_diff>
--- a/analysts.xlsx
+++ b/analysts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Nombre</t>
   </si>
@@ -73,19 +73,37 @@
   </si>
   <si>
     <t>AW0157001_Adminfo_TEST</t>
+  </si>
+  <si>
+    <t>Abel Fernando Gutierrez Arias</t>
+  </si>
+  <si>
+    <t>afgutier@bancolombia.com.co</t>
+  </si>
+  <si>
+    <t>CACT58 - Nuevos Modelos de Negocio</t>
+  </si>
+  <si>
+    <t>NU0037003_VDS_AUTOGESTIONCONSUMO_TEST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,8 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A2:XFD7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,17 +455,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
+      <c r="A2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -458,21 +479,21 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -486,21 +507,21 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -514,6 +535,20 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update para sprint 116
</commit_message>
<xml_diff>
--- a/analysts.xlsx
+++ b/analysts.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9539E7-5E61-449F-B921-C990F2B284B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{AF9539E7-5E61-449F-B921-C990F2B284B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F027AF64-C561-447F-AE6F-8FA7A2AE39C2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="118">
   <si>
     <t>Nombre</t>
   </si>
@@ -34,18 +34,6 @@
     <t>Repositorio</t>
   </si>
   <si>
-    <t>CTSEG04 - TOTH</t>
-  </si>
-  <si>
-    <t>Juan David Londono Agudelo</t>
-  </si>
-  <si>
-    <t>jdlondon@bancolombia.com.co</t>
-  </si>
-  <si>
-    <t>TCCAN09 - THE DREAM TEAM</t>
-  </si>
-  <si>
     <t>AW1259001_SucursalVirtual_Inversiones_Test</t>
   </si>
   <si>
@@ -55,33 +43,18 @@
     <t>Alex Alberto Franco Cano</t>
   </si>
   <si>
-    <t>aafranco@bancolombia.com.co</t>
-  </si>
-  <si>
-    <t>CTAP05 - ATLAS</t>
-  </si>
-  <si>
     <t>AW1294001_PCC-Portal_Conciliacion_y_Cobranza_Test</t>
   </si>
   <si>
     <t>Abel Fernando Gutierrez Arias</t>
   </si>
   <si>
-    <t>afgutier@bancolombia.com.co</t>
-  </si>
-  <si>
-    <t>CACT58 - Nuevos Modelos de Negocio</t>
-  </si>
-  <si>
     <t>Natalia Pelaez Arboleda</t>
   </si>
   <si>
     <t>npelaez@bancolombia.com.co</t>
   </si>
   <si>
-    <t>BPM07 - FLASH</t>
-  </si>
-  <si>
     <t>AW1176001_BIZAGIECUCOL_TEST</t>
   </si>
   <si>
@@ -109,30 +82,12 @@
     <t>Yuly Tatiana Murillo Cossio</t>
   </si>
   <si>
-    <t>ytmurill@bancolombia.com.co</t>
-  </si>
-  <si>
-    <t>CCAN89 - PLUG</t>
-  </si>
-  <si>
-    <t>mpzunig@bancolombia.com.co</t>
-  </si>
-  <si>
     <t>AW1010001_CreditoHipotecario_TEST</t>
   </si>
   <si>
-    <t>Damian Fernando Vengoechea Hoyos</t>
-  </si>
-  <si>
-    <t>dvengoec@bancolombia.com.co</t>
-  </si>
-  <si>
     <t>AW0360007_SVE_PortalLibranzas_Front_Test</t>
   </si>
   <si>
-    <t>Mildred Perez Zuniga</t>
-  </si>
-  <si>
     <t>Jesus Augusto Aguilar</t>
   </si>
   <si>
@@ -169,9 +124,6 @@
     <t>Mayra Alejandra Villamizar Guerrero</t>
   </si>
   <si>
-    <t>CACT13 - GANESH TEAM</t>
-  </si>
-  <si>
     <t>CTRIS02 - DREAM TEAM ECOSISTEMA</t>
   </si>
   <si>
@@ -196,12 +148,6 @@
     <t>AW0278001_SVP_TEST</t>
   </si>
   <si>
-    <t>TRANSV01 - MASNoFE</t>
-  </si>
-  <si>
-    <t>NU0089001_MODULO_ADM_SNF_Test</t>
-  </si>
-  <si>
     <t>CCAN113 - MATRIX</t>
   </si>
   <si>
@@ -413,6 +359,21 @@
   </si>
   <si>
     <t>ablando@bancolombia.com.co</t>
+  </si>
+  <si>
+    <t>BPM15 - ITZEL</t>
+  </si>
+  <si>
+    <t>CTSEG07 - APOLO</t>
+  </si>
+  <si>
+    <t>Willian Emilio Perez Castaneda</t>
+  </si>
+  <si>
+    <t>CACT13 - GANESH</t>
+  </si>
+  <si>
+    <t>wieperez@bancolombia.com.co</t>
   </si>
 </sst>
 </file>
@@ -537,13 +498,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -577,11 +537,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -590,12 +547,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -936,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:D21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -966,436 +932,324 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>77</v>
+        <v>23</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
+      <c r="A3" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>67</v>
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>129</v>
+      <c r="A4" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>80</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>53</v>
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2" t="s">
         <v>51</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>70</v>
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" t="s">
-        <v>57</v>
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>24</v>
+        <v>113</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
+      <c r="A23" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="2" t="s">
-        <v>41</v>
+      <c r="A24" s="15" t="s">
+        <v>115</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>64</v>
+        <v>116</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1405,30 +1259,31 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" xr:uid="{16C6AD1B-C9FA-4972-A7D8-436AF08D0CCE}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{6C5E22A3-C835-4FD6-8BB3-F17F303A17C6}"/>
-    <hyperlink ref="B31" r:id="rId3" xr:uid="{EF4BE9ED-827B-478F-8C38-22C23B93BC58}"/>
-    <hyperlink ref="B25" r:id="rId4" xr:uid="{762BC589-6D0C-429D-9935-4ABEBDE5FAF9}"/>
-    <hyperlink ref="B24" r:id="rId5" xr:uid="{D776301D-24C9-4091-9BB1-DE413C98AD90}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{E28B5538-00EB-4C64-9D84-A07C1D2A6C60}"/>
-    <hyperlink ref="B11" r:id="rId7" xr:uid="{8C94304F-6E9A-4FDB-BA19-43CB105403E8}"/>
-    <hyperlink ref="B12" r:id="rId8" xr:uid="{75DBEBCB-8498-40B5-BE0F-0CCC7CAEA221}"/>
-    <hyperlink ref="D24" r:id="rId9" display="https://grupobancolombia.visualstudio.com/Vicepresidencia Servicios de Tecnolog%C3%ADa/_git/AW0660001_Delfin_Test?path=%2F&amp;version=GBtrunk" xr:uid="{38D85B1D-F04B-4D8F-9843-A322C5F38BAD}"/>
-    <hyperlink ref="B29" r:id="rId10" xr:uid="{9A80B089-DBA5-4335-9E6B-626D447775E1}"/>
-    <hyperlink ref="B30" r:id="rId11" xr:uid="{4FFEF4DB-915A-4D58-9978-B9A07BEE034E}"/>
-    <hyperlink ref="B8" r:id="rId12" xr:uid="{E7855FC7-60AC-4C74-B53F-EF712867ED3E}"/>
-    <hyperlink ref="B17" r:id="rId13" xr:uid="{D531F0AB-6C5F-449E-B1B1-635F9FE6EBC3}"/>
-    <hyperlink ref="B18" r:id="rId14" xr:uid="{3192F640-8661-4136-BA9E-B7029574925D}"/>
-    <hyperlink ref="B13" r:id="rId15" xr:uid="{59F8C12F-E7D8-432C-8DAA-8A6B5C4B3180}"/>
-    <hyperlink ref="B14" r:id="rId16" xr:uid="{AD254602-E54A-4BFC-8B1B-34AA1467FDF3}"/>
-    <hyperlink ref="B15" r:id="rId17" xr:uid="{6B578A61-521D-4A0D-A3CB-E18A32CF5F51}"/>
-    <hyperlink ref="B16" r:id="rId18" xr:uid="{6193AF3B-62AD-45CF-817A-B7B0D9FF69B9}"/>
-    <hyperlink ref="B21" r:id="rId19" xr:uid="{1A418EE9-7712-4B49-888A-3E6ADF58381F}"/>
-    <hyperlink ref="B26" r:id="rId20" xr:uid="{FC4F0F31-4349-4AEE-ABE5-8AE49B013449}"/>
-    <hyperlink ref="B4" r:id="rId21" xr:uid="{BEC1A6B0-45E8-4EB0-B2DE-10531EE4BE63}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{16C6AD1B-C9FA-4972-A7D8-436AF08D0CCE}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{6C5E22A3-C835-4FD6-8BB3-F17F303A17C6}"/>
+    <hyperlink ref="B22" r:id="rId3" xr:uid="{EF4BE9ED-827B-478F-8C38-22C23B93BC58}"/>
+    <hyperlink ref="B17" r:id="rId4" xr:uid="{762BC589-6D0C-429D-9935-4ABEBDE5FAF9}"/>
+    <hyperlink ref="B16" r:id="rId5" xr:uid="{D776301D-24C9-4091-9BB1-DE413C98AD90}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{8C94304F-6E9A-4FDB-BA19-43CB105403E8}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{75DBEBCB-8498-40B5-BE0F-0CCC7CAEA221}"/>
+    <hyperlink ref="D16" r:id="rId8" display="https://grupobancolombia.visualstudio.com/Vicepresidencia Servicios de Tecnolog%C3%ADa/_git/AW0660001_Delfin_Test?path=%2F&amp;version=GBtrunk" xr:uid="{38D85B1D-F04B-4D8F-9843-A322C5F38BAD}"/>
+    <hyperlink ref="B20" r:id="rId9" xr:uid="{9A80B089-DBA5-4335-9E6B-626D447775E1}"/>
+    <hyperlink ref="B21" r:id="rId10" xr:uid="{4FFEF4DB-915A-4D58-9978-B9A07BEE034E}"/>
+    <hyperlink ref="B3" r:id="rId11" xr:uid="{E7855FC7-60AC-4C74-B53F-EF712867ED3E}"/>
+    <hyperlink ref="B11" r:id="rId12" xr:uid="{D531F0AB-6C5F-449E-B1B1-635F9FE6EBC3}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{3192F640-8661-4136-BA9E-B7029574925D}"/>
+    <hyperlink ref="B7" r:id="rId14" xr:uid="{59F8C12F-E7D8-432C-8DAA-8A6B5C4B3180}"/>
+    <hyperlink ref="B8" r:id="rId15" xr:uid="{AD254602-E54A-4BFC-8B1B-34AA1467FDF3}"/>
+    <hyperlink ref="B9" r:id="rId16" xr:uid="{6B578A61-521D-4A0D-A3CB-E18A32CF5F51}"/>
+    <hyperlink ref="B10" r:id="rId17" xr:uid="{6193AF3B-62AD-45CF-817A-B7B0D9FF69B9}"/>
+    <hyperlink ref="B15" r:id="rId18" xr:uid="{1A418EE9-7712-4B49-888A-3E6ADF58381F}"/>
+    <hyperlink ref="B18" r:id="rId19" xr:uid="{FC4F0F31-4349-4AEE-ABE5-8AE49B013449}"/>
+    <hyperlink ref="B2" r:id="rId20" xr:uid="{BEC1A6B0-45E8-4EB0-B2DE-10531EE4BE63}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{BD5B75F5-4607-4B23-8CDD-6EB1738AB41A}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{F03D62FD-D832-4BD9-937A-61AA6EC49A12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -1447,417 +1302,428 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="105" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" customHeight="1">
+      <c r="A3" s="9"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45">
+      <c r="A4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30">
+      <c r="A5" s="20"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="75">
+      <c r="A6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60">
+      <c r="A7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E8" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45">
+      <c r="A9" s="20"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="6" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="20"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105" customHeight="1">
-      <c r="A2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="16" t="s">
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="20"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45">
+      <c r="A12" s="20"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="16" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="20"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45">
+      <c r="A14" s="20"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="6" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="45">
+      <c r="A15" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="75" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45">
-      <c r="A4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="16" t="s">
+      <c r="D15" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="16"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="6" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="24"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="75">
-      <c r="A6" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
+      <c r="E17" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45">
+      <c r="A18" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="D18" s="20" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="60">
-      <c r="A7" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="20"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="6" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="60">
+      <c r="A20" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="16" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="16" t="s">
+      <c r="D20" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60">
+      <c r="A21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45">
-      <c r="A9" s="16"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="16"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="6" t="s">
+      <c r="E22" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="21" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="16"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45">
-      <c r="A12" s="16"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="6" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="45">
-      <c r="A13" s="16"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45">
-      <c r="A14" s="16"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="6" t="s">
+      <c r="D23" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45">
+      <c r="A24" s="22"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45">
+      <c r="A25" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="45">
-      <c r="A15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="16" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D25" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E25" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="60">
+      <c r="A26" s="11" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="17"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="60">
-      <c r="A17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E26" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45">
+      <c r="A27" s="17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="45">
-      <c r="A18" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="16" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D27" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="16"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="6" t="s">
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="18"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60">
-      <c r="A20" s="6" t="s">
+    <row r="29" spans="1:5" ht="45">
+      <c r="A29" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60">
+      <c r="A30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="60">
-      <c r="A21" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="E30" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60">
+      <c r="A31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30">
-      <c r="A22" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9" t="s">
+      <c r="E31" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="6" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="60">
+      <c r="A32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30">
-      <c r="A23" s="22" t="s">
+      <c r="D32" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45">
-      <c r="A24" s="23"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45">
-      <c r="A25" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="60">
-      <c r="A26" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45">
-      <c r="A27" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30">
-      <c r="A28" s="20"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="45">
-      <c r="A29" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="60">
-      <c r="A30" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="60">
-      <c r="A31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="60">
-      <c r="A32" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>64</v>
+      <c r="E32" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="C8:C14"/>
+    <mergeCell ref="D8:D14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
@@ -1867,17 +1733,6 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="C8:C14"/>
-    <mergeCell ref="D8:D14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E22" r:id="rId1" display="https://grupobancolombia.visualstudio.com/Vicepresidencia Servicios de Tecnolog%C3%ADa/_git/AW0660001_Delfin_Test?path=%2F&amp;version=GBtrunk" xr:uid="{5DFEEE1D-6CB0-477D-B1D3-84C9F5562CB2}"/>

</xml_diff>